<commit_message>
regional standard forest unit sql review
</commit_message>
<xml_diff>
--- a/scripts/Provincial_Tools/tbl_spp.xlsx
+++ b/scripts/Provincial_Tools/tbl_spp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\git\p3t_ArcGIS_Pro_Tools\scripts\SPCOMP_n_SFU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\git\p3t_ArcGIS_Pro_Tools\scripts\Provincial_Tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1517C5CE-AB00-483C-A6C7-05FF93591EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EBA3EA5-711C-414E-A586-43FA956A0EFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="instruction" sheetId="3" r:id="rId1"/>
@@ -2482,7 +2482,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2626,12 +2626,6 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
@@ -3188,7 +3182,7 @@
     </tableColumn>
     <tableColumn id="6" xr3:uid="{D68129D7-B99C-4F64-86C2-81E54A39E558}" name="Comments"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleDark1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -3500,7 +3494,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E2F87D7-D9FE-4D3B-BF72-BDA824B4466E}">
   <dimension ref="A1:A22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
@@ -3563,10 +3557,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:G122"/>
   <sheetViews>
-    <sheetView topLeftCell="A87" workbookViewId="0">
-      <selection sqref="A1:C122"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3576,7 +3573,7 @@
     <col min="4" max="4" width="34.140625" customWidth="1"/>
     <col min="5" max="5" width="12.5703125" customWidth="1"/>
     <col min="6" max="6" width="10.28515625" customWidth="1"/>
-    <col min="7" max="7" width="72.42578125" customWidth="1"/>
+    <col min="7" max="7" width="27" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3619,7 +3616,7 @@
         <v>2</v>
       </c>
       <c r="F2" t="b">
-        <f>EXACT(B2,C2)</f>
+        <f t="shared" ref="F2:F33" si="0">EXACT(B2,C2)</f>
         <v>1</v>
       </c>
     </row>
@@ -3640,7 +3637,7 @@
         <v>4</v>
       </c>
       <c r="F3" t="b">
-        <f>EXACT(B3,C3)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3661,7 +3658,7 @@
         <v>7</v>
       </c>
       <c r="F4" t="b">
-        <f>EXACT(B4,C4)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3682,7 +3679,7 @@
         <v>7</v>
       </c>
       <c r="F5" t="b">
-        <f>EXACT(B5,C5)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3703,7 +3700,7 @@
         <v>7</v>
       </c>
       <c r="F6" t="b">
-        <f>EXACT(B6,C6)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3724,7 +3721,7 @@
         <v>4</v>
       </c>
       <c r="F7" t="b">
-        <f>EXACT(B7,C7)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3745,7 +3742,7 @@
         <v>4</v>
       </c>
       <c r="F8" t="b">
-        <f>EXACT(B8,C8)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3766,7 +3763,7 @@
         <v>16</v>
       </c>
       <c r="F9" t="b">
-        <f>EXACT(B9,C9)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3787,7 +3784,7 @@
         <v>7</v>
       </c>
       <c r="F10" t="b">
-        <f>EXACT(B10,C10)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3808,7 +3805,7 @@
         <v>7</v>
       </c>
       <c r="F11" t="b">
-        <f>EXACT(B11,C11)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3829,7 +3826,7 @@
         <v>20</v>
       </c>
       <c r="F12" t="b">
-        <f>EXACT(B12,C12)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3850,7 +3847,7 @@
         <v>22</v>
       </c>
       <c r="F13" t="b">
-        <f>EXACT(B13,C13)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3871,7 +3868,7 @@
         <v>16</v>
       </c>
       <c r="F14" t="b">
-        <f>EXACT(B14,C14)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3892,7 +3889,7 @@
         <v>24</v>
       </c>
       <c r="F15" t="b">
-        <f>EXACT(B15,C15)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3913,7 +3910,7 @@
         <v>20</v>
       </c>
       <c r="F16" t="b">
-        <f>EXACT(B16,C16)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3934,7 +3931,7 @@
         <v>7</v>
       </c>
       <c r="F17" t="b">
-        <f>EXACT(B17,C17)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3955,7 +3952,7 @@
         <v>7</v>
       </c>
       <c r="F18" t="b">
-        <f>EXACT(B18,C18)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3976,7 +3973,7 @@
         <v>24</v>
       </c>
       <c r="F19" t="b">
-        <f>EXACT(B19,C19)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -3997,7 +3994,7 @@
         <v>30</v>
       </c>
       <c r="F20" t="b">
-        <f>EXACT(B20,C20)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4018,7 +4015,7 @@
         <v>7</v>
       </c>
       <c r="F21" t="b">
-        <f>EXACT(B21,C21)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4039,7 +4036,7 @@
         <v>33</v>
       </c>
       <c r="F22" t="b">
-        <f>EXACT(B22,C22)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4060,7 +4057,7 @@
         <v>7</v>
       </c>
       <c r="F23" t="b">
-        <f>EXACT(B23,C23)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4081,7 +4078,7 @@
         <v>7</v>
       </c>
       <c r="F24" t="b">
-        <f>EXACT(B24,C24)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4102,7 +4099,7 @@
         <v>37</v>
       </c>
       <c r="F25" t="b">
-        <f>EXACT(B25,C25)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4123,7 +4120,7 @@
         <v>33</v>
       </c>
       <c r="F26" t="b">
-        <f>EXACT(B26,C26)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4144,7 +4141,7 @@
         <v>33</v>
       </c>
       <c r="F27" t="b">
-        <f>EXACT(B27,C27)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4165,7 +4162,7 @@
         <v>33</v>
       </c>
       <c r="F28" t="b">
-        <f>EXACT(B28,C28)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4186,7 +4183,7 @@
         <v>7</v>
       </c>
       <c r="F29" t="b">
-        <f>EXACT(B29,C29)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4207,7 +4204,7 @@
         <v>37</v>
       </c>
       <c r="F30" t="b">
-        <f>EXACT(B30,C30)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4228,7 +4225,7 @@
         <v>7</v>
       </c>
       <c r="F31" t="b">
-        <f>EXACT(B31,C31)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4249,7 +4246,7 @@
         <v>7</v>
       </c>
       <c r="F32" t="b">
-        <f>EXACT(B32,C32)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4270,7 +4267,7 @@
         <v>37</v>
       </c>
       <c r="F33" t="b">
-        <f>EXACT(B33,C33)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -4291,7 +4288,7 @@
         <v>48</v>
       </c>
       <c r="F34" t="b">
-        <f>EXACT(B34,C34)</f>
+        <f t="shared" ref="F34:F65" si="1">EXACT(B34,C34)</f>
         <v>0</v>
       </c>
     </row>
@@ -4312,7 +4309,7 @@
         <v>7</v>
       </c>
       <c r="F35" t="b">
-        <f>EXACT(B35,C35)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -4333,7 +4330,7 @@
         <v>48</v>
       </c>
       <c r="F36" t="b">
-        <f>EXACT(B36,C36)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -4354,7 +4351,7 @@
         <v>48</v>
       </c>
       <c r="F37" t="b">
-        <f>EXACT(B37,C37)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -4375,7 +4372,7 @@
         <v>48</v>
       </c>
       <c r="F38" t="b">
-        <f>EXACT(B38,C38)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -4396,7 +4393,7 @@
         <v>48</v>
       </c>
       <c r="F39" t="b">
-        <f>EXACT(B39,C39)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -4417,7 +4414,7 @@
         <v>7</v>
       </c>
       <c r="F40" t="b">
-        <f>EXACT(B40,C40)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4438,7 +4435,7 @@
         <v>7</v>
       </c>
       <c r="F41" t="b">
-        <f>EXACT(B41,C41)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4459,7 +4456,7 @@
         <v>7</v>
       </c>
       <c r="F42" t="b">
-        <f>EXACT(B42,C42)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4480,7 +4477,7 @@
         <v>7</v>
       </c>
       <c r="F43" t="b">
-        <f>EXACT(B43,C43)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4501,7 +4498,7 @@
         <v>7</v>
       </c>
       <c r="F44" t="b">
-        <f>EXACT(B44,C44)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4522,7 +4519,7 @@
         <v>7</v>
       </c>
       <c r="F45" t="b">
-        <f>EXACT(B45,C45)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4543,7 +4540,7 @@
         <v>61</v>
       </c>
       <c r="F46" t="b">
-        <f>EXACT(B46,C46)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4564,7 +4561,7 @@
         <v>7</v>
       </c>
       <c r="F47" t="b">
-        <f>EXACT(B47,C47)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4585,7 +4582,7 @@
         <v>7</v>
       </c>
       <c r="F48" t="b">
-        <f>EXACT(B48,C48)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4606,7 +4603,7 @@
         <v>7</v>
       </c>
       <c r="F49" t="b">
-        <f>EXACT(B49,C49)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4627,7 +4624,7 @@
         <v>66</v>
       </c>
       <c r="F50" t="b">
-        <f>EXACT(B50,C50)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G50" t="s">
@@ -4651,7 +4648,7 @@
         <v>66</v>
       </c>
       <c r="F51" t="b">
-        <f>EXACT(B51,C51)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G51" t="s">
@@ -4675,7 +4672,7 @@
         <v>66</v>
       </c>
       <c r="F52" t="b">
-        <f>EXACT(B52,C52)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G52" t="s">
@@ -4699,7 +4696,7 @@
         <v>7</v>
       </c>
       <c r="F53" t="b">
-        <f>EXACT(B53,C53)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4720,7 +4717,7 @@
         <v>72</v>
       </c>
       <c r="F54" t="b">
-        <f>EXACT(B54,C54)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4741,7 +4738,7 @@
         <v>72</v>
       </c>
       <c r="F55" t="b">
-        <f>EXACT(B55,C55)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4762,7 +4759,7 @@
         <v>72</v>
       </c>
       <c r="F56" t="b">
-        <f>EXACT(B56,C56)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4783,7 +4780,7 @@
         <v>7</v>
       </c>
       <c r="F57" t="b">
-        <f>EXACT(B57,C57)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4804,7 +4801,7 @@
         <v>77</v>
       </c>
       <c r="F58" t="b">
-        <f>EXACT(B58,C58)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4825,7 +4822,7 @@
         <v>77</v>
       </c>
       <c r="F59" t="b">
-        <f>EXACT(B59,C59)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4846,7 +4843,7 @@
         <v>7</v>
       </c>
       <c r="F60" t="b">
-        <f>EXACT(B60,C60)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4867,7 +4864,7 @@
         <v>77</v>
       </c>
       <c r="F61" t="b">
-        <f>EXACT(B61,C61)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4888,7 +4885,7 @@
         <v>77</v>
       </c>
       <c r="F62" t="b">
-        <f>EXACT(B62,C62)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4909,7 +4906,7 @@
         <v>7</v>
       </c>
       <c r="F63" t="b">
-        <f>EXACT(B63,C63)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4930,7 +4927,7 @@
         <v>7</v>
       </c>
       <c r="F64" t="b">
-        <f>EXACT(B64,C64)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4951,7 +4948,7 @@
         <v>84</v>
       </c>
       <c r="F65" t="b">
-        <f>EXACT(B65,C65)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -4972,7 +4969,7 @@
         <v>84</v>
       </c>
       <c r="F66" t="b">
-        <f>EXACT(B66,C66)</f>
+        <f t="shared" ref="F66:F97" si="2">EXACT(B66,C66)</f>
         <v>1</v>
       </c>
     </row>
@@ -4993,7 +4990,7 @@
         <v>84</v>
       </c>
       <c r="F67" t="b">
-        <f>EXACT(B67,C67)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5014,7 +5011,7 @@
         <v>84</v>
       </c>
       <c r="F68" t="b">
-        <f>EXACT(B68,C68)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5035,7 +5032,7 @@
         <v>84</v>
       </c>
       <c r="F69" t="b">
-        <f>EXACT(B69,C69)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5056,7 +5053,7 @@
         <v>7</v>
       </c>
       <c r="F70" t="b">
-        <f>EXACT(B70,C70)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5077,7 +5074,7 @@
         <v>7</v>
       </c>
       <c r="F71" t="b">
-        <f>EXACT(B71,C71)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5098,7 +5095,7 @@
         <v>93</v>
       </c>
       <c r="F72" t="b">
-        <f>EXACT(B72,C72)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -5119,7 +5116,7 @@
         <v>93</v>
       </c>
       <c r="F73" t="b">
-        <f>EXACT(B73,C73)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -5140,7 +5137,7 @@
         <v>7</v>
       </c>
       <c r="F74" t="b">
-        <f>EXACT(B74,C74)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5161,7 +5158,7 @@
         <v>84</v>
       </c>
       <c r="F75" t="b">
-        <f>EXACT(B75,C75)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5182,7 +5179,7 @@
         <v>99</v>
       </c>
       <c r="F76" t="b">
-        <f>EXACT(B76,C76)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5203,7 +5200,7 @@
         <v>101</v>
       </c>
       <c r="F77" t="b">
-        <f>EXACT(B77,C77)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5224,7 +5221,7 @@
         <v>101</v>
       </c>
       <c r="F78" t="b">
-        <f>EXACT(B78,C78)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5245,7 +5242,7 @@
         <v>104</v>
       </c>
       <c r="F79" t="b">
-        <f>EXACT(B79,C79)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5266,7 +5263,7 @@
         <v>106</v>
       </c>
       <c r="F80" t="b">
-        <f>EXACT(B80,C80)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -5287,7 +5284,7 @@
         <v>7</v>
       </c>
       <c r="F81" t="b">
-        <f>EXACT(B81,C81)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5308,7 +5305,7 @@
         <v>106</v>
       </c>
       <c r="F82" t="b">
-        <f>EXACT(B82,C82)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5329,7 +5326,7 @@
         <v>99</v>
       </c>
       <c r="F83" t="b">
-        <f>EXACT(B83,C83)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5350,7 +5347,7 @@
         <v>106</v>
       </c>
       <c r="F84" t="b">
-        <f>EXACT(B84,C84)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5371,7 +5368,7 @@
         <v>106</v>
       </c>
       <c r="F85" t="b">
-        <f>EXACT(B85,C85)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5392,7 +5389,7 @@
         <v>106</v>
       </c>
       <c r="F86" t="b">
-        <f>EXACT(B86,C86)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5413,7 +5410,7 @@
         <v>99</v>
       </c>
       <c r="F87" t="b">
-        <f>EXACT(B87,C87)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5434,7 +5431,7 @@
         <v>7</v>
       </c>
       <c r="F88" t="b">
-        <f>EXACT(B88,C88)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5455,7 +5452,7 @@
         <v>118</v>
       </c>
       <c r="F89" t="b">
-        <f>EXACT(B89,C89)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -5476,7 +5473,7 @@
         <v>117</v>
       </c>
       <c r="F90" t="b">
-        <f>EXACT(B90,C90)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5497,7 +5494,7 @@
         <v>117</v>
       </c>
       <c r="F91" t="b">
-        <f>EXACT(B91,C91)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5518,7 +5515,7 @@
         <v>117</v>
       </c>
       <c r="F92" t="b">
-        <f>EXACT(B92,C92)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5539,7 +5536,7 @@
         <v>117</v>
       </c>
       <c r="F93" t="b">
-        <f>EXACT(B93,C93)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5560,7 +5557,7 @@
         <v>117</v>
       </c>
       <c r="F94" t="b">
-        <f>EXACT(B94,C94)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5581,7 +5578,7 @@
         <v>126</v>
       </c>
       <c r="F95" t="b">
-        <f>EXACT(B95,C95)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5602,7 +5599,7 @@
         <v>128</v>
       </c>
       <c r="F96" t="b">
-        <f>EXACT(B96,C96)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G96" t="s">
@@ -5626,7 +5623,7 @@
         <v>104</v>
       </c>
       <c r="F97" t="b">
-        <f>EXACT(B97,C97)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5647,7 +5644,7 @@
         <v>117</v>
       </c>
       <c r="F98" t="b">
-        <f>EXACT(B98,C98)</f>
+        <f t="shared" ref="F98:F122" si="3">EXACT(B98,C98)</f>
         <v>1</v>
       </c>
     </row>
@@ -5668,7 +5665,7 @@
         <v>104</v>
       </c>
       <c r="F99" t="b">
-        <f>EXACT(B99,C99)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -5689,7 +5686,7 @@
         <v>133</v>
       </c>
       <c r="F100" t="b">
-        <f>EXACT(B100,C100)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -5710,7 +5707,7 @@
         <v>104</v>
       </c>
       <c r="F101" t="b">
-        <f>EXACT(B101,C101)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -5731,7 +5728,7 @@
         <v>136</v>
       </c>
       <c r="F102" t="b">
-        <f>EXACT(B102,C102)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G102" t="s">
@@ -5755,7 +5752,7 @@
         <v>138</v>
       </c>
       <c r="F103" t="b">
-        <f>EXACT(B103,C103)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -5776,7 +5773,7 @@
         <v>138</v>
       </c>
       <c r="F104" t="b">
-        <f>EXACT(B104,C104)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -5797,7 +5794,7 @@
         <v>99</v>
       </c>
       <c r="F105" t="b">
-        <f>EXACT(B105,C105)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -5818,7 +5815,7 @@
         <v>7</v>
       </c>
       <c r="F106" t="b">
-        <f>EXACT(B106,C106)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -5839,7 +5836,7 @@
         <v>145</v>
       </c>
       <c r="F107" t="b">
-        <f>EXACT(B107,C107)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -5860,7 +5857,7 @@
         <v>147</v>
       </c>
       <c r="F108" t="b">
-        <f>EXACT(B108,C108)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -5881,7 +5878,7 @@
         <v>104</v>
       </c>
       <c r="F109" t="b">
-        <f>EXACT(B109,C109)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -5902,7 +5899,7 @@
         <v>104</v>
       </c>
       <c r="F110" t="b">
-        <f>EXACT(B110,C110)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -5923,7 +5920,7 @@
         <v>145</v>
       </c>
       <c r="F111" t="b">
-        <f>EXACT(B111,C111)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
@@ -5944,7 +5941,7 @@
         <v>147</v>
       </c>
       <c r="F112" t="b">
-        <f>EXACT(B112,C112)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -5965,7 +5962,7 @@
         <v>145</v>
       </c>
       <c r="F113" t="b">
-        <f>EXACT(B113,C113)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -5986,7 +5983,7 @@
         <v>7</v>
       </c>
       <c r="F114" t="b">
-        <f>EXACT(B114,C114)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -6007,7 +6004,7 @@
         <v>145</v>
       </c>
       <c r="F115" t="b">
-        <f>EXACT(B115,C115)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -6028,7 +6025,7 @@
         <v>147</v>
       </c>
       <c r="F116" t="b">
-        <f>EXACT(B116,C116)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -6049,7 +6046,7 @@
         <v>7</v>
       </c>
       <c r="F117" t="b">
-        <f>EXACT(B117,C117)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -6070,7 +6067,7 @@
         <v>77</v>
       </c>
       <c r="F118" t="b">
-        <f>EXACT(B118,C118)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -6091,7 +6088,7 @@
         <v>7</v>
       </c>
       <c r="F119" t="b">
-        <f>EXACT(B119,C119)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -6112,7 +6109,7 @@
         <v>7</v>
       </c>
       <c r="F120" t="b">
-        <f>EXACT(B120,C120)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -6133,7 +6130,7 @@
         <v>7</v>
       </c>
       <c r="F121" t="b">
-        <f>EXACT(B121,C121)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -6154,19 +6151,19 @@
         <v>30</v>
       </c>
       <c r="F122" t="b">
-        <f>EXACT(B122,C122)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="21" type="noConversion"/>
+  <phoneticPr fontId="20" type="noConversion"/>
   <conditionalFormatting sqref="F2:F122 G96 G102">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="53" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
     <tablePart r:id="rId3"/>

</xml_diff>

<commit_message>
once again updated tbl_sql_classify excel and csv
</commit_message>
<xml_diff>
--- a/scripts/Provincial_Tools/tbl_spp.xlsx
+++ b/scripts/Provincial_Tools/tbl_spp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\git\p3t_ArcGIS_Pro_Tools\scripts\Provincial_Tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\T\git\p3t_ArcGIS_Pro_Tools\scripts\Provincial_Tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EBA3EA5-711C-414E-A586-43FA956A0EFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A0602E-8A60-4088-AEEC-B737C0221562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25080" yWindow="960" windowWidth="21600" windowHeight="13680" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="instruction" sheetId="3" r:id="rId1"/>
@@ -3078,14 +3078,14 @@
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3166,10 +3166,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6A75024F-AE2F-4B42-B85F-B4FE83673C54}" name="Table1" displayName="Table1" ref="A1:G122" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6A75024F-AE2F-4B42-B85F-B4FE83673C54}" name="Table1" displayName="Table1" ref="A1:G122" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A1:G122" xr:uid="{6A75024F-AE2F-4B42-B85F-B4FE83673C54}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G122">
-    <sortCondition ref="A1:A122"/>
+    <sortCondition ref="B1:B122"/>
   </sortState>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{26E629A8-B0C2-4566-ADFF-2FE827013921}" name="spc"/>
@@ -3187,9 +3187,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3227,7 +3227,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3333,7 +3333,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3475,7 +3475,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3563,16 +3563,16 @@
   <dimension ref="A1:G122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="34.140625" customWidth="1"/>
     <col min="5" max="5" width="12.5703125" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="27" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3643,19 +3643,19 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F4" t="b">
         <f t="shared" si="0"/>
@@ -3664,19 +3664,19 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>169</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F5" t="b">
         <f t="shared" si="0"/>
@@ -3685,19 +3685,19 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="F6" t="b">
         <f t="shared" si="0"/>
@@ -3706,19 +3706,19 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>173</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="F7" t="b">
         <f t="shared" si="0"/>
@@ -3727,19 +3727,19 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E8" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="F8" t="b">
         <f t="shared" si="0"/>
@@ -3769,19 +3769,19 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>170</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E10" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="F10" t="b">
         <f t="shared" si="0"/>
@@ -3790,19 +3790,19 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="E11" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="F11" t="b">
         <f t="shared" si="0"/>
@@ -3811,19 +3811,19 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="E12" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="F12" t="b">
         <f t="shared" si="0"/>
@@ -3832,19 +3832,19 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="D13" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="E13" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="F13" t="b">
         <f t="shared" si="0"/>
@@ -3853,19 +3853,19 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>184</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="E14" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="F14" t="b">
         <f t="shared" si="0"/>
@@ -3874,19 +3874,19 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>172</v>
+        <v>187</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="D15" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="E15" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="F15" t="b">
         <f t="shared" si="0"/>
@@ -3895,19 +3895,19 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="E16" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="F16" t="b">
         <f t="shared" si="0"/>
@@ -3916,19 +3916,19 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>174</v>
+        <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="D17" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="E17" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="F17" t="b">
         <f t="shared" si="0"/>
@@ -3937,19 +3937,19 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="D18" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E18" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="F18" t="b">
         <f t="shared" si="0"/>
@@ -3958,19 +3958,19 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>182</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="C19" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D19" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="E19" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="F19" t="b">
         <f t="shared" si="0"/>
@@ -3979,124 +3979,124 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>176</v>
+        <v>46</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="D20" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="E20" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="F20" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>177</v>
+        <v>189</v>
       </c>
       <c r="B21" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="C21" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="D21" t="s">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="E21" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="F21" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>178</v>
+        <v>190</v>
       </c>
       <c r="B22" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="C22" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="D22" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="E22" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="F22" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>179</v>
+        <v>47</v>
       </c>
       <c r="B23" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="C23" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="D23" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="E23" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="F23" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>180</v>
+        <v>48</v>
       </c>
       <c r="B24" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="C24" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="D24" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="E24" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="F24" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="B25" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="C25" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="D25" t="s">
-        <v>38</v>
+        <v>62</v>
       </c>
       <c r="E25" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="F25" t="b">
         <f t="shared" si="0"/>
@@ -4105,19 +4105,19 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="B26" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="C26" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="D26" t="s">
-        <v>39</v>
+        <v>73</v>
       </c>
       <c r="E26" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="F26" t="b">
         <f t="shared" si="0"/>
@@ -4126,19 +4126,19 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>181</v>
+        <v>74</v>
       </c>
       <c r="B27" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="C27" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="D27" t="s">
-        <v>34</v>
+        <v>73</v>
       </c>
       <c r="E27" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="F27" t="b">
         <f t="shared" si="0"/>
@@ -4147,19 +4147,19 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>182</v>
+        <v>72</v>
       </c>
       <c r="B28" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="C28" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="D28" t="s">
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="E28" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="F28" t="b">
         <f t="shared" si="0"/>
@@ -4168,19 +4168,19 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>183</v>
+        <v>76</v>
       </c>
       <c r="B29" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C29" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="D29" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="E29" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="F29" t="b">
         <f t="shared" si="0"/>
@@ -4189,19 +4189,19 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>184</v>
+        <v>77</v>
       </c>
       <c r="B30" t="s">
-        <v>37</v>
+        <v>77</v>
       </c>
       <c r="C30" t="s">
-        <v>37</v>
+        <v>77</v>
       </c>
       <c r="D30" t="s">
-        <v>42</v>
+        <v>78</v>
       </c>
       <c r="E30" t="s">
-        <v>37</v>
+        <v>77</v>
       </c>
       <c r="F30" t="b">
         <f t="shared" si="0"/>
@@ -4210,19 +4210,19 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>185</v>
+        <v>204</v>
       </c>
       <c r="B31" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C31" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="D31" t="s">
-        <v>43</v>
+        <v>80</v>
       </c>
       <c r="E31" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="F31" t="b">
         <f t="shared" si="0"/>
@@ -4231,19 +4231,19 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>186</v>
+        <v>205</v>
       </c>
       <c r="B32" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="C32" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="D32" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="E32" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="F32" t="b">
         <f t="shared" si="0"/>
@@ -4252,19 +4252,19 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>187</v>
+        <v>239</v>
       </c>
       <c r="B33" t="s">
-        <v>37</v>
+        <v>77</v>
       </c>
       <c r="C33" t="s">
-        <v>37</v>
+        <v>77</v>
       </c>
       <c r="D33" t="s">
-        <v>45</v>
+        <v>158</v>
       </c>
       <c r="E33" t="s">
-        <v>37</v>
+        <v>77</v>
       </c>
       <c r="F33" t="b">
         <f t="shared" si="0"/>
@@ -4273,187 +4273,187 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>46</v>
+        <v>208</v>
       </c>
       <c r="B34" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C34" t="s">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="D34" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="E34" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="F34" t="b">
         <f t="shared" ref="F34:F65" si="1">EXACT(B34,C34)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>188</v>
+        <v>209</v>
       </c>
       <c r="B35" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="C35" t="s">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="D35" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="E35" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="F35" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>189</v>
+        <v>84</v>
       </c>
       <c r="B36" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C36" t="s">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="D36" t="s">
-        <v>51</v>
+        <v>87</v>
       </c>
       <c r="E36" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="F36" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="B37" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C37" t="s">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="D37" t="s">
-        <v>52</v>
+        <v>88</v>
       </c>
       <c r="E37" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="F37" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>47</v>
+        <v>211</v>
       </c>
       <c r="B38" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C38" t="s">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="D38" t="s">
-        <v>49</v>
+        <v>89</v>
       </c>
       <c r="E38" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="F38" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>48</v>
+        <v>215</v>
       </c>
       <c r="B39" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="C39" t="s">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="D39" t="s">
-        <v>53</v>
+        <v>97</v>
       </c>
       <c r="E39" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="F39" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>191</v>
+        <v>93</v>
       </c>
       <c r="B40" t="s">
-        <v>7</v>
+        <v>93</v>
       </c>
       <c r="C40" t="s">
-        <v>7</v>
+        <v>92</v>
       </c>
       <c r="D40" t="s">
-        <v>54</v>
+        <v>94</v>
       </c>
       <c r="E40" t="s">
-        <v>7</v>
+        <v>93</v>
       </c>
       <c r="F40" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>192</v>
+        <v>92</v>
       </c>
       <c r="B41" t="s">
-        <v>7</v>
+        <v>93</v>
       </c>
       <c r="C41" t="s">
-        <v>7</v>
+        <v>92</v>
       </c>
       <c r="D41" t="s">
-        <v>55</v>
+        <v>95</v>
       </c>
       <c r="E41" t="s">
-        <v>7</v>
+        <v>93</v>
       </c>
       <c r="F41" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>56</v>
+        <v>101</v>
       </c>
       <c r="B42" t="s">
-        <v>7</v>
+        <v>101</v>
       </c>
       <c r="C42" t="s">
-        <v>7</v>
+        <v>101</v>
       </c>
       <c r="D42" t="s">
-        <v>57</v>
+        <v>102</v>
       </c>
       <c r="E42" t="s">
-        <v>7</v>
+        <v>101</v>
       </c>
       <c r="F42" t="b">
         <f t="shared" si="1"/>
@@ -4462,19 +4462,19 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>193</v>
+        <v>216</v>
       </c>
       <c r="B43" t="s">
-        <v>7</v>
+        <v>101</v>
       </c>
       <c r="C43" t="s">
-        <v>7</v>
+        <v>101</v>
       </c>
       <c r="D43" t="s">
-        <v>58</v>
+        <v>103</v>
       </c>
       <c r="E43" t="s">
-        <v>7</v>
+        <v>101</v>
       </c>
       <c r="F43" t="b">
         <f t="shared" si="1"/>
@@ -4483,19 +4483,19 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>194</v>
+        <v>104</v>
       </c>
       <c r="B44" t="s">
-        <v>7</v>
+        <v>104</v>
       </c>
       <c r="C44" t="s">
-        <v>7</v>
+        <v>104</v>
       </c>
       <c r="D44" t="s">
-        <v>59</v>
+        <v>105</v>
       </c>
       <c r="E44" t="s">
-        <v>7</v>
+        <v>104</v>
       </c>
       <c r="F44" t="b">
         <f t="shared" si="1"/>
@@ -4504,19 +4504,19 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>195</v>
+        <v>227</v>
       </c>
       <c r="B45" t="s">
-        <v>7</v>
+        <v>104</v>
       </c>
       <c r="C45" t="s">
-        <v>7</v>
+        <v>104</v>
       </c>
       <c r="D45" t="s">
-        <v>60</v>
+        <v>130</v>
       </c>
       <c r="E45" t="s">
-        <v>7</v>
+        <v>104</v>
       </c>
       <c r="F45" t="b">
         <f t="shared" si="1"/>
@@ -4525,19 +4525,19 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>61</v>
+        <v>228</v>
       </c>
       <c r="B46" t="s">
-        <v>61</v>
+        <v>104</v>
       </c>
       <c r="C46" t="s">
-        <v>61</v>
+        <v>104</v>
       </c>
       <c r="D46" t="s">
-        <v>62</v>
+        <v>132</v>
       </c>
       <c r="E46" t="s">
-        <v>61</v>
+        <v>104</v>
       </c>
       <c r="F46" t="b">
         <f t="shared" si="1"/>
@@ -4546,19 +4546,19 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>66</v>
+        <v>229</v>
       </c>
       <c r="B47" t="s">
-        <v>7</v>
+        <v>104</v>
       </c>
       <c r="C47" t="s">
-        <v>7</v>
+        <v>104</v>
       </c>
       <c r="D47" t="s">
-        <v>63</v>
+        <v>135</v>
       </c>
       <c r="E47" t="s">
-        <v>7</v>
+        <v>104</v>
       </c>
       <c r="F47" t="b">
         <f t="shared" si="1"/>
@@ -4567,49 +4567,49 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>196</v>
+        <v>231</v>
       </c>
       <c r="B48" t="s">
-        <v>7</v>
+        <v>104</v>
       </c>
       <c r="C48" t="s">
-        <v>7</v>
+        <v>104</v>
       </c>
       <c r="D48" t="s">
-        <v>64</v>
+        <v>149</v>
       </c>
       <c r="E48" t="s">
-        <v>7</v>
+        <v>104</v>
       </c>
       <c r="F48" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>197</v>
+        <v>232</v>
       </c>
       <c r="B49" t="s">
-        <v>7</v>
+        <v>104</v>
       </c>
       <c r="C49" t="s">
-        <v>7</v>
+        <v>104</v>
       </c>
       <c r="D49" t="s">
-        <v>65</v>
+        <v>150</v>
       </c>
       <c r="E49" t="s">
-        <v>7</v>
+        <v>104</v>
       </c>
       <c r="F49" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>198</v>
+        <v>6</v>
       </c>
       <c r="B50" t="s">
         <v>7</v>
@@ -4618,22 +4618,19 @@
         <v>7</v>
       </c>
       <c r="D50" t="s">
-        <v>67</v>
+        <v>8</v>
       </c>
       <c r="E50" t="s">
-        <v>66</v>
+        <v>7</v>
       </c>
       <c r="F50" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G50" t="s">
-        <v>804</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>199</v>
+        <v>169</v>
       </c>
       <c r="B51" t="s">
         <v>7</v>
@@ -4642,22 +4639,19 @@
         <v>7</v>
       </c>
       <c r="D51" t="s">
-        <v>68</v>
+        <v>9</v>
       </c>
       <c r="E51" t="s">
-        <v>66</v>
+        <v>7</v>
       </c>
       <c r="F51" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G51" t="s">
-        <v>804</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>200</v>
+        <v>13</v>
       </c>
       <c r="B52" t="s">
         <v>7</v>
@@ -4666,22 +4660,19 @@
         <v>7</v>
       </c>
       <c r="D52" t="s">
-        <v>69</v>
+        <v>14</v>
       </c>
       <c r="E52" t="s">
-        <v>66</v>
+        <v>7</v>
       </c>
       <c r="F52" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G52" t="s">
-        <v>804</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>201</v>
+        <v>170</v>
       </c>
       <c r="B53" t="s">
         <v>7</v>
@@ -4690,7 +4681,7 @@
         <v>7</v>
       </c>
       <c r="D53" t="s">
-        <v>70</v>
+        <v>18</v>
       </c>
       <c r="E53" t="s">
         <v>7</v>
@@ -4700,72 +4691,72 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>71</v>
+        <v>171</v>
       </c>
       <c r="B54" t="s">
-        <v>72</v>
+        <v>7</v>
       </c>
       <c r="C54" t="s">
-        <v>72</v>
+        <v>7</v>
       </c>
       <c r="D54" t="s">
-        <v>73</v>
+        <v>19</v>
       </c>
       <c r="E54" t="s">
-        <v>72</v>
+        <v>7</v>
       </c>
       <c r="F54" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>74</v>
+        <v>174</v>
       </c>
       <c r="B55" t="s">
-        <v>72</v>
+        <v>7</v>
       </c>
       <c r="C55" t="s">
-        <v>72</v>
+        <v>7</v>
       </c>
       <c r="D55" t="s">
-        <v>73</v>
+        <v>27</v>
       </c>
       <c r="E55" t="s">
-        <v>72</v>
+        <v>7</v>
       </c>
       <c r="F55" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>72</v>
+        <v>175</v>
       </c>
       <c r="B56" t="s">
-        <v>72</v>
+        <v>7</v>
       </c>
       <c r="C56" t="s">
-        <v>72</v>
+        <v>7</v>
       </c>
       <c r="D56" t="s">
-        <v>73</v>
+        <v>28</v>
       </c>
       <c r="E56" t="s">
-        <v>72</v>
+        <v>7</v>
       </c>
       <c r="F56" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>202</v>
+        <v>177</v>
       </c>
       <c r="B57" t="s">
         <v>7</v>
@@ -4774,7 +4765,7 @@
         <v>7</v>
       </c>
       <c r="D57" t="s">
-        <v>75</v>
+        <v>32</v>
       </c>
       <c r="E57" t="s">
         <v>7</v>
@@ -4784,51 +4775,51 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>76</v>
+        <v>179</v>
       </c>
       <c r="B58" t="s">
-        <v>77</v>
+        <v>7</v>
       </c>
       <c r="C58" t="s">
-        <v>77</v>
+        <v>7</v>
       </c>
       <c r="D58" t="s">
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="E58" t="s">
-        <v>77</v>
+        <v>7</v>
       </c>
       <c r="F58" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>77</v>
+        <v>180</v>
       </c>
       <c r="B59" t="s">
-        <v>77</v>
+        <v>7</v>
       </c>
       <c r="C59" t="s">
-        <v>77</v>
+        <v>7</v>
       </c>
       <c r="D59" t="s">
-        <v>78</v>
+        <v>36</v>
       </c>
       <c r="E59" t="s">
-        <v>77</v>
+        <v>7</v>
       </c>
       <c r="F59" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
       <c r="B60" t="s">
         <v>7</v>
@@ -4837,7 +4828,7 @@
         <v>7</v>
       </c>
       <c r="D60" t="s">
-        <v>79</v>
+        <v>41</v>
       </c>
       <c r="E60" t="s">
         <v>7</v>
@@ -4847,72 +4838,72 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>204</v>
+        <v>185</v>
       </c>
       <c r="B61" t="s">
-        <v>77</v>
+        <v>7</v>
       </c>
       <c r="C61" t="s">
-        <v>77</v>
+        <v>7</v>
       </c>
       <c r="D61" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="E61" t="s">
-        <v>77</v>
+        <v>7</v>
       </c>
       <c r="F61" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>205</v>
+        <v>186</v>
       </c>
       <c r="B62" t="s">
-        <v>77</v>
+        <v>7</v>
       </c>
       <c r="C62" t="s">
-        <v>77</v>
+        <v>7</v>
       </c>
       <c r="D62" t="s">
-        <v>81</v>
+        <v>44</v>
       </c>
       <c r="E62" t="s">
-        <v>77</v>
+        <v>7</v>
       </c>
       <c r="F62" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>206</v>
+        <v>188</v>
       </c>
       <c r="B63" t="s">
         <v>7</v>
       </c>
       <c r="C63" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="D63" t="s">
-        <v>82</v>
+        <v>50</v>
       </c>
       <c r="E63" t="s">
         <v>7</v>
       </c>
       <c r="F63" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>207</v>
+        <v>191</v>
       </c>
       <c r="B64" t="s">
         <v>7</v>
@@ -4921,7 +4912,7 @@
         <v>7</v>
       </c>
       <c r="D64" t="s">
-        <v>83</v>
+        <v>54</v>
       </c>
       <c r="E64" t="s">
         <v>7</v>
@@ -4931,114 +4922,114 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>208</v>
+        <v>192</v>
       </c>
       <c r="B65" t="s">
-        <v>84</v>
+        <v>7</v>
       </c>
       <c r="C65" t="s">
-        <v>84</v>
+        <v>7</v>
       </c>
       <c r="D65" t="s">
-        <v>85</v>
+        <v>55</v>
       </c>
       <c r="E65" t="s">
-        <v>84</v>
+        <v>7</v>
       </c>
       <c r="F65" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>209</v>
+        <v>56</v>
       </c>
       <c r="B66" t="s">
-        <v>84</v>
+        <v>7</v>
       </c>
       <c r="C66" t="s">
-        <v>84</v>
+        <v>7</v>
       </c>
       <c r="D66" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="E66" t="s">
-        <v>84</v>
+        <v>7</v>
       </c>
       <c r="F66" t="b">
         <f t="shared" ref="F66:F97" si="2">EXACT(B66,C66)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>84</v>
+        <v>193</v>
       </c>
       <c r="B67" t="s">
-        <v>84</v>
+        <v>7</v>
       </c>
       <c r="C67" t="s">
-        <v>84</v>
+        <v>7</v>
       </c>
       <c r="D67" t="s">
-        <v>87</v>
+        <v>58</v>
       </c>
       <c r="E67" t="s">
-        <v>84</v>
+        <v>7</v>
       </c>
       <c r="F67" t="b">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>210</v>
+        <v>194</v>
       </c>
       <c r="B68" t="s">
-        <v>84</v>
+        <v>7</v>
       </c>
       <c r="C68" t="s">
-        <v>84</v>
+        <v>7</v>
       </c>
       <c r="D68" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
       <c r="E68" t="s">
-        <v>84</v>
+        <v>7</v>
       </c>
       <c r="F68" t="b">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="B69" t="s">
-        <v>84</v>
+        <v>7</v>
       </c>
       <c r="C69" t="s">
-        <v>84</v>
+        <v>7</v>
       </c>
       <c r="D69" t="s">
-        <v>89</v>
+        <v>60</v>
       </c>
       <c r="E69" t="s">
-        <v>84</v>
+        <v>7</v>
       </c>
       <c r="F69" t="b">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>212</v>
+        <v>66</v>
       </c>
       <c r="B70" t="s">
         <v>7</v>
@@ -5047,7 +5038,7 @@
         <v>7</v>
       </c>
       <c r="D70" t="s">
-        <v>90</v>
+        <v>63</v>
       </c>
       <c r="E70" t="s">
         <v>7</v>
@@ -5057,9 +5048,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>213</v>
+        <v>196</v>
       </c>
       <c r="B71" t="s">
         <v>7</v>
@@ -5068,7 +5059,7 @@
         <v>7</v>
       </c>
       <c r="D71" t="s">
-        <v>91</v>
+        <v>64</v>
       </c>
       <c r="E71" t="s">
         <v>7</v>
@@ -5078,51 +5069,54 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>93</v>
+        <v>197</v>
       </c>
       <c r="B72" t="s">
-        <v>93</v>
+        <v>7</v>
       </c>
       <c r="C72" t="s">
-        <v>92</v>
+        <v>7</v>
       </c>
       <c r="D72" t="s">
-        <v>94</v>
+        <v>65</v>
       </c>
       <c r="E72" t="s">
-        <v>93</v>
+        <v>7</v>
       </c>
       <c r="F72" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>92</v>
+        <v>198</v>
       </c>
       <c r="B73" t="s">
-        <v>93</v>
+        <v>7</v>
       </c>
       <c r="C73" t="s">
-        <v>92</v>
+        <v>7</v>
       </c>
       <c r="D73" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="E73" t="s">
-        <v>93</v>
+        <v>66</v>
       </c>
       <c r="F73" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="G73" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
       <c r="B74" t="s">
         <v>7</v>
@@ -5131,145 +5125,151 @@
         <v>7</v>
       </c>
       <c r="D74" t="s">
-        <v>96</v>
+        <v>68</v>
       </c>
       <c r="E74" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
       <c r="F74" t="b">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G74" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="B75" t="s">
-        <v>84</v>
+        <v>7</v>
       </c>
       <c r="C75" t="s">
-        <v>84</v>
+        <v>7</v>
       </c>
       <c r="D75" t="s">
-        <v>97</v>
+        <v>69</v>
       </c>
       <c r="E75" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="F75" t="b">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G75" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>98</v>
+        <v>201</v>
       </c>
       <c r="B76" t="s">
-        <v>99</v>
+        <v>7</v>
       </c>
       <c r="C76" t="s">
-        <v>99</v>
+        <v>7</v>
       </c>
       <c r="D76" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="E76" t="s">
-        <v>99</v>
+        <v>7</v>
       </c>
       <c r="F76" t="b">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>101</v>
+        <v>202</v>
       </c>
       <c r="B77" t="s">
-        <v>101</v>
+        <v>7</v>
       </c>
       <c r="C77" t="s">
-        <v>101</v>
+        <v>7</v>
       </c>
       <c r="D77" t="s">
-        <v>102</v>
+        <v>75</v>
       </c>
       <c r="E77" t="s">
-        <v>101</v>
+        <v>7</v>
       </c>
       <c r="F77" t="b">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="B78" t="s">
-        <v>101</v>
+        <v>7</v>
       </c>
       <c r="C78" t="s">
-        <v>101</v>
+        <v>7</v>
       </c>
       <c r="D78" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
       <c r="E78" t="s">
-        <v>101</v>
+        <v>7</v>
       </c>
       <c r="F78" t="b">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>104</v>
+        <v>206</v>
       </c>
       <c r="B79" t="s">
-        <v>104</v>
+        <v>7</v>
       </c>
       <c r="C79" t="s">
-        <v>104</v>
+        <v>7</v>
       </c>
       <c r="D79" t="s">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="E79" t="s">
-        <v>104</v>
+        <v>7</v>
       </c>
       <c r="F79" t="b">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="B80" t="s">
-        <v>106</v>
+        <v>7</v>
       </c>
       <c r="C80" t="s">
-        <v>99</v>
+        <v>7</v>
       </c>
       <c r="D80" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="E80" t="s">
-        <v>106</v>
+        <v>7</v>
       </c>
       <c r="F80" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>7</v>
+        <v>212</v>
       </c>
       <c r="B81" t="s">
         <v>7</v>
@@ -5278,7 +5278,7 @@
         <v>7</v>
       </c>
       <c r="D81" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="E81" t="s">
         <v>7</v>
@@ -5288,135 +5288,135 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B82" t="s">
-        <v>106</v>
+        <v>7</v>
       </c>
       <c r="C82" t="s">
-        <v>106</v>
+        <v>7</v>
       </c>
       <c r="D82" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="E82" t="s">
-        <v>106</v>
+        <v>7</v>
       </c>
       <c r="F82" t="b">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="B83" t="s">
-        <v>99</v>
+        <v>7</v>
       </c>
       <c r="C83" t="s">
-        <v>99</v>
+        <v>7</v>
       </c>
       <c r="D83" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="E83" t="s">
-        <v>99</v>
+        <v>7</v>
       </c>
       <c r="F83" t="b">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>220</v>
+        <v>7</v>
       </c>
       <c r="B84" t="s">
-        <v>106</v>
+        <v>7</v>
       </c>
       <c r="C84" t="s">
-        <v>106</v>
+        <v>7</v>
       </c>
       <c r="D84" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E84" t="s">
-        <v>106</v>
+        <v>7</v>
       </c>
       <c r="F84" t="b">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B85" t="s">
-        <v>106</v>
+        <v>7</v>
       </c>
       <c r="C85" t="s">
-        <v>106</v>
+        <v>7</v>
       </c>
       <c r="D85" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="E85" t="s">
-        <v>106</v>
+        <v>7</v>
       </c>
       <c r="F85" t="b">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>106</v>
+        <v>230</v>
       </c>
       <c r="B86" t="s">
-        <v>106</v>
+        <v>7</v>
       </c>
       <c r="C86" t="s">
-        <v>106</v>
+        <v>7</v>
       </c>
       <c r="D86" t="s">
-        <v>113</v>
+        <v>143</v>
       </c>
       <c r="E86" t="s">
-        <v>106</v>
+        <v>7</v>
       </c>
       <c r="F86" t="b">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>114</v>
+        <v>236</v>
       </c>
       <c r="B87" t="s">
-        <v>99</v>
+        <v>7</v>
       </c>
       <c r="C87" t="s">
-        <v>99</v>
+        <v>7</v>
       </c>
       <c r="D87" t="s">
-        <v>115</v>
+        <v>154</v>
       </c>
       <c r="E87" t="s">
-        <v>99</v>
+        <v>7</v>
       </c>
       <c r="F87" t="b">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>222</v>
+        <v>238</v>
       </c>
       <c r="B88" t="s">
         <v>7</v>
@@ -5425,7 +5425,7 @@
         <v>7</v>
       </c>
       <c r="D88" t="s">
-        <v>116</v>
+        <v>157</v>
       </c>
       <c r="E88" t="s">
         <v>7</v>
@@ -5435,213 +5435,210 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>118</v>
+        <v>240</v>
       </c>
       <c r="B89" t="s">
-        <v>118</v>
+        <v>7</v>
       </c>
       <c r="C89" t="s">
-        <v>117</v>
+        <v>7</v>
       </c>
       <c r="D89" t="s">
-        <v>119</v>
+        <v>159</v>
       </c>
       <c r="E89" t="s">
-        <v>118</v>
+        <v>7</v>
       </c>
       <c r="F89" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>223</v>
+        <v>241</v>
       </c>
       <c r="B90" t="s">
-        <v>117</v>
+        <v>7</v>
       </c>
       <c r="C90" t="s">
-        <v>117</v>
+        <v>7</v>
       </c>
       <c r="D90" t="s">
-        <v>120</v>
+        <v>160</v>
       </c>
       <c r="E90" t="s">
-        <v>117</v>
+        <v>7</v>
       </c>
       <c r="F90" t="b">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>224</v>
+        <v>242</v>
       </c>
       <c r="B91" t="s">
-        <v>117</v>
+        <v>7</v>
       </c>
       <c r="C91" t="s">
-        <v>117</v>
+        <v>7</v>
       </c>
       <c r="D91" t="s">
-        <v>121</v>
+        <v>161</v>
       </c>
       <c r="E91" t="s">
-        <v>117</v>
+        <v>7</v>
       </c>
       <c r="F91" t="b">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="B92" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="C92" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="D92" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="E92" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="F92" t="b">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>123</v>
+        <v>218</v>
       </c>
       <c r="B93" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="C93" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="D93" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="E93" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="F93" t="b">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="B94" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="C94" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="D94" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="E94" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="F94" t="b">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>126</v>
+        <v>221</v>
       </c>
       <c r="B95" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="C95" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="D95" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="E95" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="F95" t="b">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="B96" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="C96" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="D96" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="E96" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="F96" t="b">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G96" t="s">
-        <v>805</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>227</v>
+        <v>118</v>
       </c>
       <c r="B97" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
       <c r="C97" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="D97" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="E97" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
       <c r="F97" t="b">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="B98" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="C98" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="D98" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E98" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="F98" t="b">
         <f t="shared" ref="F98:F122" si="3">EXACT(B98,C98)</f>
@@ -5650,40 +5647,43 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>228</v>
+        <v>128</v>
       </c>
       <c r="B99" t="s">
-        <v>104</v>
+        <v>128</v>
       </c>
       <c r="C99" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="D99" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="E99" t="s">
-        <v>104</v>
+        <v>128</v>
       </c>
       <c r="F99" t="b">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="G99" t="s">
+        <v>805</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>133</v>
+        <v>223</v>
       </c>
       <c r="B100" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="C100" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="D100" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="E100" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="F100" t="b">
         <f t="shared" si="3"/>
@@ -5692,19 +5692,19 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="B101" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="C101" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="D101" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="E101" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="F101" t="b">
         <f t="shared" si="3"/>
@@ -5713,43 +5713,40 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>136</v>
+        <v>225</v>
       </c>
       <c r="B102" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="C102" t="s">
         <v>117</v>
       </c>
       <c r="D102" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="E102" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="F102" t="b">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="G102" t="s">
-        <v>806</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="B103" t="s">
-        <v>138</v>
+        <v>117</v>
       </c>
       <c r="C103" t="s">
-        <v>138</v>
+        <v>117</v>
       </c>
       <c r="D103" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="E103" t="s">
-        <v>138</v>
+        <v>117</v>
       </c>
       <c r="F103" t="b">
         <f t="shared" si="3"/>
@@ -5758,19 +5755,19 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>140</v>
+        <v>226</v>
       </c>
       <c r="B104" t="s">
-        <v>138</v>
+        <v>117</v>
       </c>
       <c r="C104" t="s">
-        <v>138</v>
+        <v>117</v>
       </c>
       <c r="D104" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="E104" t="s">
-        <v>138</v>
+        <v>117</v>
       </c>
       <c r="F104" t="b">
         <f t="shared" si="3"/>
@@ -5779,19 +5776,19 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
       <c r="B105" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
       <c r="C105" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
       <c r="D105" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="E105" t="s">
-        <v>99</v>
+        <v>117</v>
       </c>
       <c r="F105" t="b">
         <f t="shared" si="3"/>
@@ -5800,19 +5797,19 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>230</v>
+        <v>133</v>
       </c>
       <c r="B106" t="s">
-        <v>7</v>
+        <v>133</v>
       </c>
       <c r="C106" t="s">
-        <v>7</v>
+        <v>133</v>
       </c>
       <c r="D106" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="E106" t="s">
-        <v>7</v>
+        <v>133</v>
       </c>
       <c r="F106" t="b">
         <f t="shared" si="3"/>
@@ -5821,40 +5818,43 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="B107" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C107" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
       <c r="D107" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="E107" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="F107" t="b">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="G107" t="s">
+        <v>806</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="B108" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C108" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="D108" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="E108" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="F108" t="b">
         <f t="shared" si="3"/>
@@ -5863,19 +5863,19 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>231</v>
+        <v>140</v>
       </c>
       <c r="B109" t="s">
-        <v>104</v>
+        <v>138</v>
       </c>
       <c r="C109" t="s">
-        <v>104</v>
+        <v>138</v>
       </c>
       <c r="D109" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="E109" t="s">
-        <v>104</v>
+        <v>138</v>
       </c>
       <c r="F109" t="b">
         <f t="shared" si="3"/>
@@ -5884,19 +5884,19 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>232</v>
+        <v>98</v>
       </c>
       <c r="B110" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C110" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D110" t="s">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="E110" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="F110" t="b">
         <f t="shared" si="3"/>
@@ -5905,40 +5905,40 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="B111" t="s">
-        <v>145</v>
+        <v>99</v>
       </c>
       <c r="C111" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D111" t="s">
-        <v>151</v>
+        <v>110</v>
       </c>
       <c r="E111" t="s">
-        <v>145</v>
+        <v>99</v>
       </c>
       <c r="F111" t="b">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>234</v>
+        <v>114</v>
       </c>
       <c r="B112" t="s">
-        <v>147</v>
+        <v>99</v>
       </c>
       <c r="C112" t="s">
-        <v>147</v>
+        <v>99</v>
       </c>
       <c r="D112" t="s">
-        <v>152</v>
+        <v>115</v>
       </c>
       <c r="E112" t="s">
-        <v>147</v>
+        <v>99</v>
       </c>
       <c r="F112" t="b">
         <f t="shared" si="3"/>
@@ -5947,19 +5947,19 @@
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>235</v>
+        <v>99</v>
       </c>
       <c r="B113" t="s">
-        <v>145</v>
+        <v>99</v>
       </c>
       <c r="C113" t="s">
-        <v>145</v>
+        <v>99</v>
       </c>
       <c r="D113" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="E113" t="s">
-        <v>145</v>
+        <v>99</v>
       </c>
       <c r="F113" t="b">
         <f t="shared" si="3"/>
@@ -5968,19 +5968,19 @@
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>236</v>
+        <v>147</v>
       </c>
       <c r="B114" t="s">
-        <v>7</v>
+        <v>147</v>
       </c>
       <c r="C114" t="s">
-        <v>7</v>
+        <v>147</v>
       </c>
       <c r="D114" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="E114" t="s">
-        <v>7</v>
+        <v>147</v>
       </c>
       <c r="F114" t="b">
         <f t="shared" si="3"/>
@@ -5989,19 +5989,19 @@
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>145</v>
+        <v>234</v>
       </c>
       <c r="B115" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C115" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D115" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E115" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="F115" t="b">
         <f t="shared" si="3"/>
@@ -6031,19 +6031,19 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>238</v>
+        <v>144</v>
       </c>
       <c r="B117" t="s">
-        <v>7</v>
+        <v>145</v>
       </c>
       <c r="C117" t="s">
-        <v>7</v>
+        <v>145</v>
       </c>
       <c r="D117" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="E117" t="s">
-        <v>7</v>
+        <v>145</v>
       </c>
       <c r="F117" t="b">
         <f t="shared" si="3"/>
@@ -6052,40 +6052,40 @@
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="B118" t="s">
-        <v>77</v>
+        <v>145</v>
       </c>
       <c r="C118" t="s">
-        <v>77</v>
+        <v>104</v>
       </c>
       <c r="D118" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="E118" t="s">
-        <v>77</v>
+        <v>145</v>
       </c>
       <c r="F118" t="b">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="B119" t="s">
-        <v>7</v>
+        <v>145</v>
       </c>
       <c r="C119" t="s">
-        <v>7</v>
+        <v>145</v>
       </c>
       <c r="D119" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="E119" t="s">
-        <v>7</v>
+        <v>145</v>
       </c>
       <c r="F119" t="b">
         <f t="shared" si="3"/>
@@ -6094,19 +6094,19 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>241</v>
+        <v>145</v>
       </c>
       <c r="B120" t="s">
-        <v>7</v>
+        <v>145</v>
       </c>
       <c r="C120" t="s">
-        <v>7</v>
+        <v>145</v>
       </c>
       <c r="D120" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="E120" t="s">
-        <v>7</v>
+        <v>145</v>
       </c>
       <c r="F120" t="b">
         <f t="shared" si="3"/>
@@ -6115,19 +6115,19 @@
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>242</v>
+        <v>176</v>
       </c>
       <c r="B121" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="C121" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="D121" t="s">
-        <v>161</v>
+        <v>31</v>
       </c>
       <c r="E121" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="F121" t="b">
         <f t="shared" si="3"/>
@@ -6158,7 +6158,7 @@
   </sheetData>
   <phoneticPr fontId="20" type="noConversion"/>
   <conditionalFormatting sqref="F2:F122 G96 G102">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>